<commit_message>
updated data with foreign crowdources
</commit_message>
<xml_diff>
--- a/Analysis/CrowdData/users_analysis.xlsx
+++ b/Analysis/CrowdData/users_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7485" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="126">
   <si>
     <t>M</t>
   </si>
@@ -58,36 +59,12 @@
     <t>F</t>
   </si>
   <si>
-    <t>Yorick de Vries</t>
-  </si>
-  <si>
-    <t>y.c.devries-1@student.tudelft.nl</t>
-  </si>
-  <si>
-    <t>Dutch</t>
-  </si>
-  <si>
     <t>Septian Gilang Permana Putra</t>
   </si>
   <si>
     <t>septiangilang92@gmail.com</t>
   </si>
   <si>
-    <t>Joey</t>
-  </si>
-  <si>
-    <t>j.haas-1@student.tudelft.nl</t>
-  </si>
-  <si>
-    <t>jan</t>
-  </si>
-  <si>
-    <t>j.g.zegers@student.tudelft.nl</t>
-  </si>
-  <si>
-    <t>Netherlander</t>
-  </si>
-  <si>
     <t>Qiaoqiao Li</t>
   </si>
   <si>
@@ -166,12 +143,6 @@
     <t>t.tutyarsyida@student.tudelft.nl</t>
   </si>
   <si>
-    <t>Herman</t>
-  </si>
-  <si>
-    <t>hermanb@ch.tudelft.nl</t>
-  </si>
-  <si>
     <t>Rucha Bapat</t>
   </si>
   <si>
@@ -391,10 +362,52 @@
     <t>female</t>
   </si>
   <si>
-    <t>campaign_set2</t>
-  </si>
-  <si>
     <t>ages</t>
+  </si>
+  <si>
+    <t>Pavel Kucherbaev</t>
+  </si>
+  <si>
+    <t>pavel.kucherbaev@gmail.com</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Jie Yang</t>
+  </si>
+  <si>
+    <t>j.yang-3@tudelft.nl</t>
+  </si>
+  <si>
+    <t>Achilleas Psyllidis</t>
+  </si>
+  <si>
+    <t>A.Psyllidis@tudelft.nl</t>
+  </si>
+  <si>
+    <t>Bontor Humala</t>
+  </si>
+  <si>
+    <t>BontorHumala@student.tudelft.nl</t>
+  </si>
+  <si>
+    <t>&lt; 20</t>
+  </si>
+  <si>
+    <t>&gt; 30</t>
+  </si>
+  <si>
+    <t>21-25</t>
+  </si>
+  <si>
+    <t>26-30</t>
+  </si>
+  <si>
+    <t>age range</t>
+  </si>
+  <si>
+    <t>campaign_set</t>
   </si>
 </sst>
 </file>
@@ -452,15 +465,24 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="29" formatCode="mm:ss.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="29" formatCode="mm:ss.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="29" formatCode="mm:ss.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="29" formatCode="mm:ss.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -476,16 +498,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="H2cX" refreshedDate="42948.643827777778" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="H2cX" refreshedDate="42962.547677546296" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="9">
-    <cacheField name="campaign_set" numFmtId="0">
+  <cacheFields count="10">
+    <cacheField name="user_id" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="10"/>
     </cacheField>
-    <cacheField name="user_id" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="17" maxValue="80"/>
+    <cacheField name="campaign_set2" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="14" maxValue="80"/>
     </cacheField>
     <cacheField name="name" numFmtId="0">
       <sharedItems/>
@@ -495,40 +517,49 @@
     </cacheField>
     <cacheField name="gender" numFmtId="0">
       <sharedItems count="2">
+        <s v="M"/>
         <s v="F"/>
-        <s v="M"/>
       </sharedItems>
     </cacheField>
     <cacheField name="age" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="17" maxValue="34" count="10">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="17" maxValue="34" count="12">
+        <n v="30"/>
+        <n v="27"/>
+        <n v="33"/>
         <n v="23"/>
         <n v="25"/>
-        <n v="22"/>
-        <n v="34"/>
         <n v="28"/>
         <n v="26"/>
         <n v="24"/>
-        <n v="27"/>
         <n v="29"/>
         <n v="17"/>
+        <n v="34" u="1"/>
+        <n v="22" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="ages" numFmtId="0">
+      <sharedItems count="4">
+        <s v="26-30"/>
+        <s v="&gt; 30"/>
+        <s v="21-25"/>
+        <s v="&lt; 20"/>
       </sharedItems>
     </cacheField>
     <cacheField name="nationality" numFmtId="0">
-      <sharedItems count="7">
+      <sharedItems count="6">
+        <s v="Russian"/>
+        <s v="Chinese"/>
+        <s v="Greek"/>
         <s v="Indonesian"/>
-        <s v="Dutch"/>
-        <s v="Netherlander"/>
-        <s v="Chinese"/>
         <s v="Indian"/>
         <s v="British"/>
-        <s v="Greek"/>
       </sharedItems>
     </cacheField>
     <cacheField name="start" numFmtId="47">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2017-03-27T00:27:26" maxDate="2017-05-09T01:29:28"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2017-03-26T23:10:15" maxDate="2017-05-09T01:29:28"/>
     </cacheField>
-    <cacheField name="end" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2017-03-27T01:12:56" maxDate="2017-05-09T02:12:22"/>
+    <cacheField name="end" numFmtId="47">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2017-03-26T23:48:02" maxDate="2017-05-09T02:12:22"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -543,67 +574,73 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="50">
   <r>
     <n v="3"/>
+    <n v="14"/>
+    <s v="Pavel Kucherbaev"/>
+    <s v="pavel.kucherbaev@gmail.com"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <d v="2017-03-26T23:10:15"/>
+    <d v="2017-03-26T23:52:07"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="15"/>
+    <s v="Jie Yang"/>
+    <s v="j.yang-3@tudelft.nl"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <d v="2017-03-26T23:10:30"/>
+    <d v="2017-03-27T00:01:26"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="16"/>
+    <s v="Achilleas Psyllidis"/>
+    <s v="A.Psyllidis@tudelft.nl"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <d v="2017-03-26T23:10:38"/>
+    <d v="2017-03-26T23:48:02"/>
+  </r>
+  <r>
+    <n v="3"/>
     <n v="17"/>
     <s v="dwi sasetyaningtyas"/>
     <s v="sasetyaningtyas@gmail.com"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-27T00:27:26"/>
     <d v="2017-03-27T01:12:56"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <n v="21"/>
-    <s v="Yorick de Vries"/>
-    <s v="y.c.devries-1@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <d v="2017-03-28T08:53:37"/>
-    <d v="2017-03-28T09:44:53"/>
   </r>
   <r>
     <n v="2"/>
     <n v="22"/>
     <s v="Septian Gilang Permana Putra"/>
     <s v="septiangilang92@gmail.com"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-28T10:05:53"/>
     <d v="2017-03-27T23:21:18"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <n v="23"/>
-    <s v="Joey"/>
-    <s v="j.haas-1@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <d v="2017-03-28T02:02:18"/>
-    <d v="2017-03-28T02:45:42"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <n v="24"/>
-    <s v="jan"/>
-    <s v="j.g.zegers@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="2"/>
-    <d v="2017-03-28T02:04:32"/>
-    <d v="2017-03-28T02:45:01"/>
   </r>
   <r>
     <n v="1"/>
     <n v="25"/>
     <s v="Qiaoqiao Li"/>
     <s v="q.li-5@student.tudelft.nl"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
     <d v="2017-03-28T03:13:08"/>
     <d v="2017-03-28T03:46:14"/>
   </r>
@@ -612,9 +649,10 @@
     <n v="30"/>
     <s v="Arkka Dhiratara"/>
     <s v="ArkkaDhiratara@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="4"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-28T23:29:55"/>
     <d v="2017-03-29T00:26:46"/>
   </r>
@@ -623,9 +661,10 @@
     <n v="31"/>
     <s v="Sindunuraga R. P."/>
     <s v="sindunuragarp@gmail.com"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-28T23:33:26"/>
     <d v="2017-03-29T00:27:14"/>
   </r>
@@ -634,8 +673,9 @@
     <n v="32"/>
     <s v="Shashank Prasad Rao"/>
     <s v="s.p.rao@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
     <x v="4"/>
     <d v="2017-03-28T23:33:49"/>
     <d v="2017-03-29T00:23:27"/>
@@ -645,9 +685,10 @@
     <n v="33"/>
     <s v="Bramka Arga Jafino"/>
     <s v="bramkaarga@gmail.com"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-28T23:35:23"/>
     <d v="2017-03-29T00:27:29"/>
   </r>
@@ -656,9 +697,10 @@
     <n v="35"/>
     <s v="Muhammad Ridho Rosa"/>
     <s v="muhammadridhorosa@gmail.com"/>
-    <x v="1"/>
-    <x v="5"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-28T23:46:16"/>
     <d v="2017-03-29T00:27:59"/>
   </r>
@@ -667,9 +709,10 @@
     <n v="36"/>
     <s v="helmiriawan"/>
     <s v="helmiriawan@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="5"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-28T23:47:26"/>
     <d v="2017-03-29T00:44:58"/>
   </r>
@@ -678,8 +721,9 @@
     <n v="37"/>
     <s v="Ishan Ghanmode"/>
     <s v="ishanghanmode@outlook.com"/>
-    <x v="1"/>
-    <x v="6"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="2"/>
     <x v="4"/>
     <d v="2017-03-29T00:48:43"/>
     <d v="2017-03-29T01:31:22"/>
@@ -689,9 +733,10 @@
     <n v="38"/>
     <s v="Mohamat Ulin Nuha"/>
     <s v="MohamatUlinNuha@student.tudelft.nl"/>
+    <x v="0"/>
     <x v="1"/>
-    <x v="7"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-29T00:49:00"/>
     <d v="2017-03-29T01:22:59"/>
   </r>
@@ -700,8 +745,9 @@
     <n v="39"/>
     <s v="Conrad Brown"/>
     <s v="conrad.brown42@gmail.com"/>
-    <x v="1"/>
-    <x v="4"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="0"/>
     <x v="5"/>
     <d v="2017-03-29T01:57:07"/>
     <m/>
@@ -711,9 +757,10 @@
     <n v="40"/>
     <s v="Anindito Kusumojati"/>
     <s v="anindito.kusumojati@gmail.com"/>
-    <x v="1"/>
-    <x v="5"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-29T01:57:35"/>
     <d v="2017-03-29T02:53:17"/>
   </r>
@@ -722,20 +769,22 @@
     <n v="41"/>
     <s v="T Arsyida"/>
     <s v="t.tutyarsyida@student.tudelft.nl"/>
-    <x v="0"/>
+    <x v="1"/>
     <x v="8"/>
     <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-29T01:57:55"/>
     <d v="2017-03-29T02:53:59"/>
   </r>
   <r>
     <n v="2"/>
     <n v="42"/>
-    <s v="Herman"/>
-    <s v="hermanb@ch.tudelft.nl"/>
+    <s v="Bontor Humala"/>
+    <s v="BontorHumala@student.tudelft.nl"/>
+    <x v="0"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-29T03:14:30"/>
     <d v="2017-03-29T03:58:31"/>
   </r>
@@ -744,8 +793,9 @@
     <n v="43"/>
     <s v="Rucha Bapat"/>
     <s v="r.m.bapat@student.tudelft.nl"/>
-    <x v="0"/>
     <x v="1"/>
+    <x v="4"/>
+    <x v="2"/>
     <x v="4"/>
     <d v="2017-03-29T03:14:44"/>
     <d v="2017-03-29T03:48:05"/>
@@ -755,9 +805,10 @@
     <n v="44"/>
     <s v="William Suriana"/>
     <s v="william.suriana@gmail.com"/>
-    <x v="1"/>
-    <x v="6"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-29T03:15:51"/>
     <d v="2017-03-29T04:29:14"/>
   </r>
@@ -766,8 +817,9 @@
     <n v="45"/>
     <s v="Aditi Rawat"/>
     <s v="A.rawat@student.tudelft.nl"/>
-    <x v="0"/>
-    <x v="6"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="2"/>
     <x v="4"/>
     <d v="2017-03-29T03:17:01"/>
     <d v="2017-03-29T04:02:10"/>
@@ -777,9 +829,10 @@
     <n v="47"/>
     <s v="Insani Abdi Bangsa"/>
     <s v="insaniabdi@gmail.com"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-30T08:54:22"/>
     <d v="2017-03-30T09:57:59"/>
   </r>
@@ -788,9 +841,10 @@
     <n v="48"/>
     <s v="Dimas Ramadhan Abdillah Fikri"/>
     <s v="DimasRamadhanAbdillahFikri@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-30T08:57:38"/>
     <d v="2017-03-30T09:48:55"/>
   </r>
@@ -799,9 +853,10 @@
     <n v="49"/>
     <s v="Andreas Maruli Christian Pangaribuan"/>
     <s v="andreas.mc.pangaribuan@gmail.com"/>
-    <x v="1"/>
+    <x v="0"/>
     <x v="9"/>
-    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
     <d v="2017-03-30T10:08:04"/>
     <d v="2017-03-30T10:51:05"/>
   </r>
@@ -810,9 +865,10 @@
     <n v="50"/>
     <s v="Reza Aditya Permadi"/>
     <s v="r.a.permadi@student.tudelft.nl"/>
-    <x v="1"/>
+    <x v="0"/>
     <x v="8"/>
     <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-30T10:07:53"/>
     <d v="2017-03-30T10:56:15"/>
   </r>
@@ -821,9 +877,10 @@
     <n v="51"/>
     <s v="Muhamad Zamroni"/>
     <s v="zamroni.ep07@gmail.com"/>
+    <x v="0"/>
     <x v="1"/>
-    <x v="7"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-30T10:09:36"/>
     <d v="2017-03-30T10:53:23"/>
   </r>
@@ -832,9 +889,10 @@
     <n v="52"/>
     <s v="Romi Kharisnawan"/>
     <s v="romikharisnawan@gmail.com"/>
-    <x v="1"/>
-    <x v="5"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-30T10:43:09"/>
     <d v="2017-03-29T23:17:07"/>
   </r>
@@ -843,9 +901,10 @@
     <n v="53"/>
     <s v="Vasileios Milias"/>
     <s v="milias.vasilis@gmail.com"/>
-    <x v="1"/>
-    <x v="6"/>
-    <x v="6"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="2"/>
     <d v="2017-03-30T02:03:53"/>
     <d v="2017-03-30T02:54:45"/>
   </r>
@@ -854,9 +913,10 @@
     <n v="54"/>
     <s v="Affan Kaysa Waafi"/>
     <s v="affankaysawaafi@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-30T02:05:05"/>
     <d v="2017-03-30T02:50:01"/>
   </r>
@@ -865,9 +925,10 @@
     <n v="55"/>
     <s v="Adrian Promediaz"/>
     <s v="AdrianPromediaz@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="5"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-30T02:05:00"/>
     <d v="2017-03-30T03:02:03"/>
   </r>
@@ -876,8 +937,9 @@
     <n v="56"/>
     <s v="Sambit Praharaj"/>
     <s v="sambit_praharaj@yahoo.com"/>
-    <x v="1"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
     <x v="4"/>
     <d v="2017-03-30T03:22:26"/>
     <d v="2017-03-30T04:33:14"/>
@@ -887,9 +949,10 @@
     <n v="57"/>
     <s v="Andri Rahmadhani"/>
     <s v="andrewflash@gmail.com"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-30T03:22:56"/>
     <d v="2017-03-30T04:18:29"/>
   </r>
@@ -898,9 +961,10 @@
     <n v="58"/>
     <s v="Muhammad Faris"/>
     <s v="mhmmdfrs@gmail.com"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-30T03:31:43"/>
     <d v="2017-03-30T04:30:44"/>
   </r>
@@ -909,9 +973,10 @@
     <n v="59"/>
     <s v="Atindriyo Kusumo Pamososuryo"/>
     <s v="atindriyo.kp@gmail.com"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-03-31T01:59:08"/>
     <d v="2017-03-31T02:34:05"/>
   </r>
@@ -920,9 +985,10 @@
     <n v="60"/>
     <s v="Nadia Rayhanna"/>
     <s v="nrayhanna@gmail.com"/>
-    <x v="0"/>
-    <x v="5"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-03-31T01:55:58"/>
     <d v="2017-03-31T02:54:04"/>
   </r>
@@ -931,9 +997,10 @@
     <n v="62"/>
     <s v="Dimas Ramadhan Abdillah Fikri"/>
     <s v="DimasRamadhanAbdillahFikri@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="5"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-05-01T00:49:53"/>
     <d v="2017-05-01T01:43:16"/>
   </r>
@@ -942,9 +1009,10 @@
     <n v="63"/>
     <s v="Prahesa Kusuma Setia"/>
     <s v="prahesakusumasetia@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-05-02T02:27:22"/>
     <d v="2017-05-02T03:27:21"/>
   </r>
@@ -953,9 +1021,10 @@
     <n v="64"/>
     <s v="Tulus"/>
     <s v="imaro.tulus@gmail.com"/>
-    <x v="1"/>
-    <x v="4"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-05-02T04:27:04"/>
     <d v="2017-05-02T05:00:46"/>
   </r>
@@ -964,9 +1033,10 @@
     <n v="65"/>
     <s v="Antony Rainer Mallianto Santosa"/>
     <s v="rainer.civil@gmail.com"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-05-02T04:26:56"/>
     <d v="2017-05-03T07:12:49"/>
   </r>
@@ -975,9 +1045,10 @@
     <n v="66"/>
     <s v="Andre Prakoso"/>
     <s v="andreprakoso@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-05-02T04:42:12"/>
     <d v="2017-05-02T05:29:19"/>
   </r>
@@ -986,9 +1057,10 @@
     <n v="67"/>
     <s v="Parikesit Abdi Negara"/>
     <s v="rpabdinegara@gmail.com"/>
+    <x v="0"/>
     <x v="1"/>
-    <x v="7"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-05-03T09:54:59"/>
     <d v="2017-05-03T10:43:03"/>
   </r>
@@ -997,9 +1069,10 @@
     <n v="68"/>
     <s v="Aulia Recky"/>
     <s v="AuliaReckySoepeno@student.tudelft.nl"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-05-02T23:07:53"/>
     <d v="2017-05-02T23:47:58"/>
   </r>
@@ -1008,9 +1081,10 @@
     <n v="69"/>
     <s v="Rhadityo Bhaskoro Arbarim"/>
     <s v="rhadityobhaskoro@yahoo.com"/>
-    <x v="1"/>
-    <x v="5"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-05-03T01:14:49"/>
     <d v="2017-05-03T01:50:55"/>
   </r>
@@ -1019,9 +1093,10 @@
     <n v="70"/>
     <s v="Yunizar Natanael Pragistio"/>
     <s v="yunizar.agis11@gmail.com"/>
-    <x v="1"/>
-    <x v="6"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-05-04T10:55:42"/>
     <d v="2017-05-03T23:36:24"/>
   </r>
@@ -1030,9 +1105,10 @@
     <n v="72"/>
     <s v="mustaqim"/>
     <s v="mustaaqim@gmail.com"/>
+    <x v="0"/>
     <x v="1"/>
-    <x v="7"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-05-04T02:13:48"/>
     <d v="2017-05-04T02:48:50"/>
   </r>
@@ -1041,9 +1117,10 @@
     <n v="73"/>
     <s v="Zahrina Hafizhah"/>
     <s v="zahrinahafizhah@gmail.com"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-05-04T02:24:16"/>
     <d v="2017-05-04T03:15:42"/>
   </r>
@@ -1052,9 +1129,10 @@
     <n v="75"/>
     <s v="Christian Gerald Daniel"/>
     <s v="christian.geralddaniel@gmail.com"/>
-    <x v="1"/>
-    <x v="6"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="3"/>
     <d v="2017-05-09T01:03:36"/>
     <d v="2017-05-09T01:50:01"/>
   </r>
@@ -1063,9 +1141,10 @@
     <n v="76"/>
     <s v="Hakim Agung Ramadhan"/>
     <s v="hakimagungramadhan@gmail.com"/>
-    <x v="1"/>
-    <x v="4"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-05-09T01:03:25"/>
     <d v="2017-05-09T01:54:08"/>
   </r>
@@ -1074,9 +1153,10 @@
     <n v="77"/>
     <s v="Aldy Gustinara"/>
     <s v="aldy.gustinara@gmail.com"/>
+    <x v="0"/>
     <x v="1"/>
-    <x v="7"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-05-09T01:29:28"/>
     <d v="2017-05-09T02:12:22"/>
   </r>
@@ -1085,9 +1165,10 @@
     <n v="80"/>
     <s v="pramudya arif d"/>
     <s v="pramudyaad@gmail.com"/>
-    <x v="1"/>
-    <x v="5"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="3"/>
     <d v="2017-05-04T01:04:43"/>
     <d v="2017-05-04T02:08:02"/>
   </r>
@@ -1095,44 +1176,54 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField subtotalTop="0" showAll="0"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0">
       <items count="3">
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="9"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="8"/>
-        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField subtotalTop="0" showAll="0">
-      <items count="8">
+      <items count="13">
+        <item x="9"/>
+        <item m="1" x="11"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="1"/>
         <item x="5"/>
+        <item x="8"/>
+        <item m="1" x="10"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
         <item x="3"/>
         <item x="1"/>
-        <item x="6"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
         <item x="4"/>
+        <item x="3"/>
         <item x="0"/>
-        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1140,9 +1231,9 @@
     <pivotField subtotalTop="0" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="5"/>
+    <field x="6"/>
   </rowFields>
-  <rowItems count="11">
+  <rowItems count="5">
     <i>
       <x/>
     </i>
@@ -1155,24 +1246,6 @@
     <i>
       <x v="3"/>
     </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
@@ -1181,7 +1254,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of user_id" fld="1" subtotal="count" baseField="5" baseItem="0"/>
+    <dataField name="Count of user_id" fld="0" subtotal="count" baseField="5" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1196,21 +1269,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J51" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J52" totalsRowCount="1">
   <autoFilter ref="A1:J51"/>
+  <sortState ref="A2:J51">
+    <sortCondition ref="A1:A51"/>
+  </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" name="user_id"/>
-    <tableColumn id="10" name="campaign_set2"/>
+    <tableColumn id="2" name="campaign_set"/>
+    <tableColumn id="10" name="user_id"/>
     <tableColumn id="3" name="name"/>
     <tableColumn id="4" name="email"/>
     <tableColumn id="5" name="gender"/>
-    <tableColumn id="6" name="age"/>
-    <tableColumn id="11" name="ages" dataDxfId="0">
+    <tableColumn id="6" name="age" totalsRowFunction="custom">
+      <totalsRowFormula>AVERAGE(Table1[age])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="11" name="ages" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="nationality"/>
-    <tableColumn id="8" name="start" dataDxfId="2"/>
-    <tableColumn id="9" name="end" dataDxfId="1"/>
+    <tableColumn id="8" name="start" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="9" name="end" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1513,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B14"/>
+  <dimension ref="A3:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="A4:B13"/>
+      <selection activeCell="A4" sqref="A4:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,97 +1607,49 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>17</v>
+      <c r="A4" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>22</v>
+      <c r="A5" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="4">
         <v>23</v>
       </c>
-      <c r="B6" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>24</v>
-      </c>
-      <c r="B7" s="4">
-        <v>6</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>25</v>
+      <c r="A8" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="B8" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>27</v>
-      </c>
-      <c r="B10" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>28</v>
-      </c>
-      <c r="B11" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>29</v>
-      </c>
-      <c r="B12" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>34</v>
-      </c>
-      <c r="B13" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="4">
         <v>50</v>
       </c>
     </row>
@@ -1630,10 +1660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,48 +1675,48 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" t="s">
         <v>110</v>
       </c>
-      <c r="F1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" t="s">
-        <v>121</v>
-      </c>
       <c r="H1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="J1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>25</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -1694,7 +1724,7 @@
       <c r="F2">
         <v>23</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G2" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -1710,16 +1740,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>39</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -1727,29 +1757,30 @@
       <c r="F3">
         <v>28</v>
       </c>
-      <c r="G3" t="str">
+      <c r="G3" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1">
         <v>42823.081331018519</v>
       </c>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>40</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -1757,7 +1788,7 @@
       <c r="F4">
         <v>26</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G4" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -1773,16 +1804,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>41</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -1790,7 +1821,7 @@
       <c r="F5">
         <v>29</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -1806,16 +1837,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>60</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -1823,7 +1854,7 @@
       <c r="F6">
         <v>26</v>
       </c>
-      <c r="G6" t="str">
+      <c r="G6" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -1839,16 +1870,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
         <v>22</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
@@ -1856,7 +1887,7 @@
       <c r="F7">
         <v>25</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G7" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -1872,29 +1903,29 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
         <v>42</v>
       </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>25</v>
-      </c>
-      <c r="G8" t="str">
-        <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
-        <v>21-25</v>
+        <v>27</v>
+      </c>
+      <c r="G8" s="4" t="str">
+        <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
+        <v>26-30</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
         <v>42823.135069444441</v>
@@ -1905,16 +1936,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
         <v>43</v>
       </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -1922,12 +1953,12 @@
       <c r="F9">
         <v>25</v>
       </c>
-      <c r="G9" t="str">
+      <c r="G9" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I9" s="1">
         <v>42823.135231481479</v>
@@ -1938,16 +1969,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
         <v>44</v>
       </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
@@ -1955,7 +1986,7 @@
       <c r="F10">
         <v>24</v>
       </c>
-      <c r="G10" t="str">
+      <c r="G10" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -1971,16 +2002,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
         <v>45</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -1988,12 +2019,12 @@
       <c r="F11">
         <v>24</v>
       </c>
-      <c r="G11" t="str">
+      <c r="G11" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I11" s="1">
         <v>42823.136817129627</v>
@@ -2004,148 +2035,148 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>23</v>
-      </c>
-      <c r="G12" t="str">
-        <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
-        <v>21-25</v>
+        <v>30</v>
+      </c>
+      <c r="G12" s="4" t="str">
+        <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
+        <v>26-30</v>
       </c>
       <c r="H12" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="I12" s="1">
-        <v>42821.019050925926</v>
+        <v>42820.965451388889</v>
       </c>
       <c r="J12" s="1">
-        <v>42821.05064814815</v>
+        <v>42820.994525462964</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>25</v>
-      </c>
-      <c r="G13" t="str">
-        <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
-        <v>21-25</v>
+        <v>27</v>
+      </c>
+      <c r="G13" s="4" t="str">
+        <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
+        <v>26-30</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="I13" s="1">
-        <v>42822.370567129627</v>
+        <v>42820.965624999997</v>
       </c>
       <c r="J13" s="1">
-        <v>42822.406168981484</v>
+        <v>42821.00099537037</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>22</v>
-      </c>
-      <c r="G14" t="str">
-        <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
-        <v>21-25</v>
+        <v>33</v>
+      </c>
+      <c r="G14" s="4" t="str">
+        <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
+        <v>&gt; 30</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I14" s="1">
-        <v>42822.084930555553</v>
+        <v>42820.965717592589</v>
       </c>
       <c r="J14" s="1">
-        <v>42822.115069444444</v>
+        <v>42820.991689814815</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F15">
-        <v>34</v>
-      </c>
-      <c r="G15" t="str">
-        <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
-        <v>&gt; 30</v>
+        <v>23</v>
+      </c>
+      <c r="G15" s="4" t="str">
+        <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
+        <v>21-25</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1">
-        <v>42822.086481481485</v>
+        <v>42821.019050925926</v>
       </c>
       <c r="J15" s="1">
-        <v>42822.114594907405</v>
+        <v>42821.05064814815</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
         <v>58</v>
       </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
@@ -2153,7 +2184,7 @@
       <c r="F16">
         <v>25</v>
       </c>
-      <c r="G16" t="str">
+      <c r="G16" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2169,16 +2200,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
         <v>49</v>
       </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
@@ -2186,7 +2217,7 @@
       <c r="F17">
         <v>17</v>
       </c>
-      <c r="G17" t="str">
+      <c r="G17" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>&lt; 20</v>
       </c>
@@ -2202,16 +2233,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
         <v>50</v>
       </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
         <v>0</v>
@@ -2219,7 +2250,7 @@
       <c r="F18">
         <v>29</v>
       </c>
-      <c r="G18" t="str">
+      <c r="G18" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -2235,16 +2266,16 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
         <v>51</v>
       </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
         <v>0</v>
@@ -2252,7 +2283,7 @@
       <c r="F19">
         <v>27</v>
       </c>
-      <c r="G19" t="str">
+      <c r="G19" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -2268,16 +2299,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
         <v>52</v>
       </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
@@ -2285,7 +2316,7 @@
       <c r="F20">
         <v>26</v>
       </c>
-      <c r="G20" t="str">
+      <c r="G20" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -2301,16 +2332,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
         <v>59</v>
       </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
         <v>0</v>
@@ -2318,7 +2349,7 @@
       <c r="F21">
         <v>25</v>
       </c>
-      <c r="G21" t="str">
+      <c r="G21" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2334,16 +2365,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
         <v>30</v>
       </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
@@ -2351,7 +2382,7 @@
       <c r="F22">
         <v>28</v>
       </c>
-      <c r="G22" t="str">
+      <c r="G22" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -2367,16 +2398,16 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
         <v>31</v>
       </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
@@ -2384,7 +2415,7 @@
       <c r="F23">
         <v>23</v>
       </c>
-      <c r="G23" t="str">
+      <c r="G23" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2400,16 +2431,16 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
         <v>32</v>
       </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E24" t="s">
         <v>0</v>
@@ -2417,12 +2448,12 @@
       <c r="F24">
         <v>25</v>
       </c>
-      <c r="G24" t="str">
+      <c r="G24" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
       <c r="H24" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I24" s="1">
         <v>42822.981817129628</v>
@@ -2433,16 +2464,16 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
         <v>33</v>
       </c>
-      <c r="B25">
-        <v>5</v>
-      </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E25" t="s">
         <v>0</v>
@@ -2450,7 +2481,7 @@
       <c r="F25">
         <v>23</v>
       </c>
-      <c r="G25" t="str">
+      <c r="G25" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2466,16 +2497,16 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
         <v>36</v>
       </c>
-      <c r="B26">
-        <v>5</v>
-      </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E26" t="s">
         <v>0</v>
@@ -2483,7 +2514,7 @@
       <c r="F26">
         <v>26</v>
       </c>
-      <c r="G26" t="str">
+      <c r="G26" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -2499,16 +2530,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
         <v>35</v>
       </c>
-      <c r="B27">
-        <v>6</v>
-      </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E27" t="s">
         <v>0</v>
@@ -2516,7 +2547,7 @@
       <c r="F27">
         <v>26</v>
       </c>
-      <c r="G27" t="str">
+      <c r="G27" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -2532,16 +2563,16 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28">
         <v>37</v>
       </c>
-      <c r="B28">
-        <v>6</v>
-      </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s">
         <v>0</v>
@@ -2549,12 +2580,12 @@
       <c r="F28">
         <v>24</v>
       </c>
-      <c r="G28" t="str">
+      <c r="G28" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
       <c r="H28" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I28" s="1">
         <v>42823.033831018518</v>
@@ -2565,16 +2596,16 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
         <v>38</v>
       </c>
-      <c r="B29">
-        <v>6</v>
-      </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
         <v>0</v>
@@ -2582,7 +2613,7 @@
       <c r="F29">
         <v>27</v>
       </c>
-      <c r="G29" t="str">
+      <c r="G29" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -2598,16 +2629,16 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30">
         <v>47</v>
       </c>
-      <c r="B30">
-        <v>6</v>
-      </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
         <v>0</v>
@@ -2615,7 +2646,7 @@
       <c r="F30">
         <v>23</v>
       </c>
-      <c r="G30" t="str">
+      <c r="G30" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2631,16 +2662,16 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31">
         <v>48</v>
       </c>
-      <c r="B31">
-        <v>6</v>
-      </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E31" t="s">
         <v>0</v>
@@ -2648,7 +2679,7 @@
       <c r="F31">
         <v>25</v>
       </c>
-      <c r="G31" t="str">
+      <c r="G31" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2664,16 +2695,16 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32">
         <v>53</v>
       </c>
-      <c r="B32">
-        <v>7</v>
-      </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E32" t="s">
         <v>0</v>
@@ -2681,7 +2712,7 @@
       <c r="F32">
         <v>24</v>
       </c>
-      <c r="G32" t="str">
+      <c r="G32" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2697,16 +2728,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33">
         <v>54</v>
       </c>
-      <c r="B33">
-        <v>7</v>
-      </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
         <v>0</v>
@@ -2714,7 +2745,7 @@
       <c r="F33">
         <v>25</v>
       </c>
-      <c r="G33" t="str">
+      <c r="G33" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2730,16 +2761,16 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34">
         <v>55</v>
       </c>
-      <c r="B34">
-        <v>7</v>
-      </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
         <v>0</v>
@@ -2747,7 +2778,7 @@
       <c r="F34">
         <v>26</v>
       </c>
-      <c r="G34" t="str">
+      <c r="G34" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -2763,16 +2794,16 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35">
         <v>56</v>
       </c>
-      <c r="B35">
-        <v>7</v>
-      </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E35" t="s">
         <v>0</v>
@@ -2780,12 +2811,12 @@
       <c r="F35">
         <v>23</v>
       </c>
-      <c r="G35" t="str">
+      <c r="G35" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
       <c r="H35" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I35" s="1">
         <v>42824.1405787037</v>
@@ -2796,16 +2827,16 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36">
         <v>57</v>
       </c>
-      <c r="B36">
-        <v>7</v>
-      </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E36" t="s">
         <v>0</v>
@@ -2813,7 +2844,7 @@
       <c r="F36">
         <v>25</v>
       </c>
-      <c r="G36" t="str">
+      <c r="G36" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2829,16 +2860,16 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37">
         <v>63</v>
       </c>
-      <c r="B37">
-        <v>8</v>
-      </c>
       <c r="C37" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E37" t="s">
         <v>0</v>
@@ -2846,7 +2877,7 @@
       <c r="F37">
         <v>25</v>
       </c>
-      <c r="G37" t="str">
+      <c r="G37" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2862,16 +2893,16 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
+        <v>8</v>
+      </c>
+      <c r="B38">
         <v>64</v>
       </c>
-      <c r="B38">
-        <v>8</v>
-      </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E38" t="s">
         <v>0</v>
@@ -2879,7 +2910,7 @@
       <c r="F38">
         <v>28</v>
       </c>
-      <c r="G38" t="str">
+      <c r="G38" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -2895,16 +2926,16 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39">
         <v>65</v>
       </c>
-      <c r="B39">
-        <v>8</v>
-      </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
         <v>0</v>
@@ -2912,7 +2943,7 @@
       <c r="F39">
         <v>25</v>
       </c>
-      <c r="G39" t="str">
+      <c r="G39" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2928,16 +2959,16 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40">
         <v>66</v>
       </c>
-      <c r="B40">
-        <v>8</v>
-      </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D40" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E40" t="s">
         <v>0</v>
@@ -2945,7 +2976,7 @@
       <c r="F40">
         <v>23</v>
       </c>
-      <c r="G40" t="str">
+      <c r="G40" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -2961,16 +2992,16 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
+        <v>8</v>
+      </c>
+      <c r="B41">
         <v>67</v>
       </c>
-      <c r="B41">
-        <v>8</v>
-      </c>
       <c r="C41" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D41" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E41" t="s">
         <v>0</v>
@@ -2978,7 +3009,7 @@
       <c r="F41">
         <v>27</v>
       </c>
-      <c r="G41" t="str">
+      <c r="G41" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -2994,16 +3025,16 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
+        <v>9</v>
+      </c>
+      <c r="B42">
         <v>68</v>
       </c>
-      <c r="B42">
-        <v>9</v>
-      </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E42" t="s">
         <v>0</v>
@@ -3011,7 +3042,7 @@
       <c r="F42">
         <v>23</v>
       </c>
-      <c r="G42" t="str">
+      <c r="G42" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -3027,16 +3058,16 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43">
         <v>69</v>
       </c>
-      <c r="B43">
-        <v>9</v>
-      </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D43" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E43" t="s">
         <v>0</v>
@@ -3044,7 +3075,7 @@
       <c r="F43">
         <v>26</v>
       </c>
-      <c r="G43" t="str">
+      <c r="G43" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -3060,16 +3091,16 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44">
         <v>72</v>
       </c>
-      <c r="B44">
-        <v>9</v>
-      </c>
       <c r="C44" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E44" t="s">
         <v>0</v>
@@ -3077,7 +3108,7 @@
       <c r="F44">
         <v>27</v>
       </c>
-      <c r="G44" t="str">
+      <c r="G44" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -3093,16 +3124,16 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45">
         <v>73</v>
       </c>
-      <c r="B45">
-        <v>9</v>
-      </c>
       <c r="C45" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -3110,7 +3141,7 @@
       <c r="F45">
         <v>23</v>
       </c>
-      <c r="G45" t="str">
+      <c r="G45" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -3126,16 +3157,16 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46">
         <v>80</v>
       </c>
-      <c r="B46">
-        <v>9</v>
-      </c>
       <c r="C46" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D46" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E46" t="s">
         <v>0</v>
@@ -3143,7 +3174,7 @@
       <c r="F46">
         <v>26</v>
       </c>
-      <c r="G46" t="str">
+      <c r="G46" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -3159,16 +3190,16 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
+        <v>10</v>
+      </c>
+      <c r="B47">
         <v>62</v>
       </c>
-      <c r="B47">
-        <v>10</v>
-      </c>
       <c r="C47" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E47" t="s">
         <v>0</v>
@@ -3176,7 +3207,7 @@
       <c r="F47">
         <v>26</v>
       </c>
-      <c r="G47" t="str">
+      <c r="G47" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -3192,16 +3223,16 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
+        <v>10</v>
+      </c>
+      <c r="B48">
         <v>70</v>
       </c>
-      <c r="B48">
-        <v>10</v>
-      </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E48" t="s">
         <v>0</v>
@@ -3209,7 +3240,7 @@
       <c r="F48">
         <v>24</v>
       </c>
-      <c r="G48" t="str">
+      <c r="G48" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -3225,16 +3256,16 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
+        <v>10</v>
+      </c>
+      <c r="B49">
         <v>75</v>
       </c>
-      <c r="B49">
-        <v>10</v>
-      </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D49" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E49" t="s">
         <v>0</v>
@@ -3242,7 +3273,7 @@
       <c r="F49">
         <v>24</v>
       </c>
-      <c r="G49" t="str">
+      <c r="G49" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>21-25</v>
       </c>
@@ -3258,16 +3289,16 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50">
         <v>76</v>
       </c>
-      <c r="B50">
-        <v>10</v>
-      </c>
       <c r="C50" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D50" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E50" t="s">
         <v>0</v>
@@ -3275,7 +3306,7 @@
       <c r="F50">
         <v>28</v>
       </c>
-      <c r="G50" t="str">
+      <c r="G50" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -3291,10 +3322,10 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51">
         <v>77</v>
-      </c>
-      <c r="B51">
-        <v>10</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -3308,7 +3339,7 @@
       <c r="F51">
         <v>27</v>
       </c>
-      <c r="G51" t="str">
+      <c r="G51" s="4" t="str">
         <f>IF(Table1[[#This Row],[age]]&lt;=20,"&lt; 20",IF(Table1[[#This Row],[age]]&lt;=25,"21-25",IF(Table1[[#This Row],[age]]&lt;=30,"26-30","&gt; 30")))</f>
         <v>26-30</v>
       </c>
@@ -3320,6 +3351,21 @@
       </c>
       <c r="J51" s="1">
         <v>42864.091921296298</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f>AVERAGE(Table1[age])</f>
+        <v>25.48</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f>_xlfn.STDEV.P(Table1[age])</f>
+        <v>2.4019991673603887</v>
       </c>
     </row>
   </sheetData>
@@ -3332,17 +3378,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B1">
         <f>43/50</f>
@@ -3351,7 +3397,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B2">
         <f>1-B1</f>
@@ -3360,7 +3406,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -3375,16 +3421,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" ref="C9:C14" si="0">B9/50</f>
-        <v>0.02</v>
+        <f t="shared" ref="C9:C13" si="0">B9/50</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
@@ -3396,50 +3442,96 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4">
         <v>5</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B12" s="4">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="B13" s="4">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" si="0"/>
-        <v>0.76</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="4">
-        <v>2</v>
-      </c>
-      <c r="C14" s="5">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <f>B16/SUM($B$16:$B$19)</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5">
+        <f>B17/SUM($B$16:$B$19)</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18" s="5">
+        <f>B18/SUM($B$16:$B$19)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19">
+        <v>23</v>
+      </c>
+      <c r="C19" s="5">
+        <f>B19/SUM($B$16:$B$19)</f>
+        <v>0.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>